<commit_message>
New directory layout. Added nearest_icao_finder.
</commit_message>
<xml_diff>
--- a/data/Checklists nominal.xlsx
+++ b/data/Checklists nominal.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABEACE02EC53F31C599C5BDE589D" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D8D1086F-B55C-4B68-A092-AC8318C24B51}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_F25DC773A252ABEACE02EC53F31C599C5BDE589D" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{04A4321F-399C-4E7D-8518-F249BA7EABCA}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,10 +602,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>43759.647037037001</v>
+        <v>43466.647037037037</v>
       </c>
       <c r="C2" s="2">
-        <v>43759.6478935185</v>
+        <v>43466.647893518515</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -850,8 +850,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045D28EA33B1D374F90B741F2AF73533E" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3358440ca6a3098c284a1e565a0f249">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d6e80eea-1699-4de5-969f-0d9eb2724e77" xmlns:ns3="4de5569b-e040-4e3a-896c-3d10ceee17bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb47b5338ca8491327e26f4cc584ed1f" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045D28EA33B1D374F90B741F2AF73533E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70f0338854bc56f50ac4daf9a6be0e17">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d6e80eea-1699-4de5-969f-0d9eb2724e77" xmlns:ns3="4de5569b-e040-4e3a-896c-3d10ceee17bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88fb165263e20f462f96975fe477339d" ns2:_="" ns3:_="">
     <xsd:import namespace="d6e80eea-1699-4de5-969f-0d9eb2724e77"/>
     <xsd:import namespace="4de5569b-e040-4e3a-896c-3d10ceee17bb"/>
     <xsd:element name="properties">
@@ -869,6 +878,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -912,6 +922,13 @@
     <xsd:element name="MediaServiceLocation" ma:index="14" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1044,15 +1061,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1060,13 +1068,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EF67ACA-907C-47F3-9652-E45A37D6C96F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9490256D-FE71-47F1-BF3D-91D2AB4FCEA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9490256D-FE71-47F1-BF3D-91D2AB4FCEA7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097F2E4-7E29-4DBF-8D28-2AAE2A62041F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8A07314-A218-4DF1-BCBF-9D26657E292F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8A07314-A218-4DF1-BCBF-9D26657E292F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>